<commit_message>
Code in a new style
</commit_message>
<xml_diff>
--- a/Docs/bom.xlsx
+++ b/Docs/bom.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="43">
   <si>
     <t>Wat</t>
   </si>
@@ -101,9 +101,6 @@
     <t>DS2E-ML2-DC5V</t>
   </si>
   <si>
-    <t>47µF 35V</t>
-  </si>
-  <si>
     <t>Display</t>
   </si>
   <si>
@@ -150,6 +147,12 @@
   </si>
   <si>
     <t>33K</t>
+  </si>
+  <si>
+    <t>47µF 16V</t>
+  </si>
+  <si>
+    <t>CH28-2032LF</t>
   </si>
 </sst>
 </file>
@@ -205,10 +208,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
@@ -494,15 +496,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="12.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
     <col min="6" max="6" width="12.85546875" customWidth="1"/>
@@ -548,10 +550,10 @@
       <c r="E2">
         <v>2</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>0.86</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <f>E2*F2</f>
         <v>1.72</v>
       </c>
@@ -567,24 +569,24 @@
         <v>21</v>
       </c>
       <c r="D3">
-        <v>2068686</v>
+        <v>9695907</v>
       </c>
       <c r="E3">
-        <v>10</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.121</v>
-      </c>
-      <c r="G3" s="4">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="G3" s="3">
         <f t="shared" ref="G3:G22" si="0">E3*F3</f>
-        <v>1.21</v>
+        <v>0.6</v>
       </c>
       <c r="K3" t="s">
         <v>8</v>
       </c>
-      <c r="L3" s="3">
-        <f>SUM(G2:G22)</f>
-        <v>51.331000000000003</v>
+      <c r="L3" s="2">
+        <f>SUM(G2:G22)*1.21</f>
+        <v>28.616499999999991</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
@@ -595,20 +597,20 @@
         <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="D4">
-        <v>2079246</v>
+        <v>1850100</v>
       </c>
       <c r="E4">
-        <v>10</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.71</v>
-      </c>
-      <c r="G4" s="4">
-        <f t="shared" si="0"/>
-        <v>7.1</v>
+        <v>2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.27</v>
+      </c>
+      <c r="G4" s="3">
+        <f t="shared" si="0"/>
+        <v>0.54</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -627,10 +629,10 @@
       <c r="E5">
         <v>4</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>0.105</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <f t="shared" si="0"/>
         <v>0.42</v>
       </c>
@@ -651,14 +653,14 @@
       <c r="E6">
         <v>2</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>5.88</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -677,10 +679,10 @@
       <c r="E7">
         <v>2</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>4.0199999999999996</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>8.0399999999999991</v>
       </c>
@@ -699,14 +701,14 @@
         <v>1650680</v>
       </c>
       <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="F8" s="4">
+        <v>1</v>
+      </c>
+      <c r="F8" s="3">
         <v>1.45</v>
       </c>
-      <c r="G8" s="4">
-        <f t="shared" si="0"/>
-        <v>2.9</v>
+      <c r="G8" s="3">
+        <f t="shared" si="0"/>
+        <v>1.45</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -723,25 +725,25 @@
         <v>2215653</v>
       </c>
       <c r="E9">
-        <v>5</v>
-      </c>
-      <c r="F9" s="4">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="G9" s="4">
-        <f t="shared" si="0"/>
-        <v>0.35000000000000003</v>
+      <c r="G9" s="3">
+        <f t="shared" si="0"/>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
       </c>
       <c r="D10">
         <v>1771725</v>
@@ -749,23 +751,23 @@
       <c r="E10">
         <v>5</v>
       </c>
-      <c r="F10" s="4">
-        <v>1.8200000000000001E-2</v>
-      </c>
-      <c r="G10" s="4">
-        <f t="shared" si="0"/>
-        <v>9.0999999999999998E-2</v>
+      <c r="F10" s="3">
+        <v>0.182</v>
+      </c>
+      <c r="G10" s="3">
+        <f t="shared" si="0"/>
+        <v>0.90999999999999992</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C11" t="s">
         <v>29</v>
-      </c>
-      <c r="C11" t="s">
-        <v>30</v>
       </c>
       <c r="D11">
         <v>9102981</v>
@@ -773,190 +775,210 @@
       <c r="E11">
         <v>5</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>0.41</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>2.0499999999999998</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>33</v>
-      </c>
-      <c r="C12" t="s">
-        <v>34</v>
       </c>
       <c r="E12">
         <v>2</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4">
+      <c r="F12" s="3"/>
+      <c r="G12" s="3">
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="B13" t="s">
         <v>35</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>36</v>
+      </c>
+      <c r="D13">
+        <v>1362552</v>
       </c>
       <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13" s="4">
-        <v>18.420000000000002</v>
-      </c>
-      <c r="G13" s="4">
-        <f t="shared" si="0"/>
-        <v>18.420000000000002</v>
+        <v>10</v>
+      </c>
+      <c r="F13" s="3">
+        <v>2.7E-2</v>
+      </c>
+      <c r="G13" s="3">
+        <f>E13*F13</f>
+        <v>0.27</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>6</v>
+        <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D14">
-        <v>1362552</v>
+        <v>9725253</v>
       </c>
       <c r="E14">
-        <v>10</v>
-      </c>
-      <c r="F14" s="4">
-        <v>2.7E-2</v>
-      </c>
-      <c r="G14" s="4">
-        <f t="shared" si="0"/>
-        <v>0.27</v>
+        <v>1</v>
+      </c>
+      <c r="F14" s="3">
+        <v>3.4</v>
+      </c>
+      <c r="G14" s="3">
+        <f>E14*F14</f>
+        <v>3.4</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D15">
-        <v>9725253</v>
+        <v>1612522</v>
       </c>
       <c r="E15">
-        <v>2</v>
-      </c>
-      <c r="F15" s="4">
-        <v>3.4</v>
-      </c>
-      <c r="G15" s="4">
-        <f t="shared" si="0"/>
-        <v>6.8</v>
+        <v>20</v>
+      </c>
+      <c r="F15" s="3">
+        <v>2.3E-2</v>
+      </c>
+      <c r="G15" s="3">
+        <f>E15*F15</f>
+        <v>0.45999999999999996</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
         <v>40</v>
       </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
       <c r="D16">
-        <v>1612522</v>
+        <v>1738979</v>
       </c>
       <c r="E16">
-        <v>20</v>
-      </c>
-      <c r="F16" s="4">
-        <v>2.3E-2</v>
-      </c>
-      <c r="G16" s="4">
-        <f t="shared" si="0"/>
-        <v>0.45999999999999996</v>
+        <v>25</v>
+      </c>
+      <c r="F16" s="3">
+        <v>0.06</v>
+      </c>
+      <c r="G16" s="3">
+        <f>E16*F16</f>
+        <v>1.5</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D17">
-        <v>1738979</v>
+        <v>2064725</v>
       </c>
       <c r="E17">
-        <v>25</v>
-      </c>
-      <c r="F17" s="4">
-        <v>0.06</v>
-      </c>
-      <c r="G17" s="4">
-        <f t="shared" si="0"/>
-        <v>1.5</v>
+        <v>5</v>
+      </c>
+      <c r="F17" s="3">
+        <v>0.43</v>
+      </c>
+      <c r="G17" s="3">
+        <f>E17*F17</f>
+        <v>2.15</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F18" s="4"/>
-      <c r="G18" s="4">
+      <c r="F18" s="3"/>
+      <c r="G18" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F19" s="4"/>
-      <c r="G19" s="4">
+      <c r="F19" s="3"/>
+      <c r="G19" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F20" s="4"/>
-      <c r="G20" s="4">
+      <c r="F20" s="3"/>
+      <c r="G20" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F21" s="4"/>
-      <c r="G21" s="4">
+      <c r="F21" s="3"/>
+      <c r="G21" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F22" s="4"/>
-      <c r="G22" s="4">
+      <c r="F22" s="3"/>
+      <c r="G22" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="A23" t="s">
+        <v>34</v>
+      </c>
+      <c r="B23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23" s="3">
+        <v>18.420000000000002</v>
+      </c>
+      <c r="G23" s="3">
+        <f>E23*F23</f>
+        <v>18.420000000000002</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>